<commit_message>
Released version, with 4mils/4mils for track width and isolation on outer and inner layers 0.45mm for inner and outer annular ring 0.1mm for finished via drill (for Seeed studio increase to 0.2mm) + USB connector added
</commit_message>
<xml_diff>
--- a/hardware/udriver3/Fab/uOmodri_BOM.xlsx
+++ b/hardware/udriver3/Fab/uOmodri_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmanhes\LAAS\Actionneur\OMODRI\hardware\udriver3\Fab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676FD6A8-A143-4B95-BA53-9E2D1DA5BFC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5126BD37-1E1D-48B4-8E73-4D4BF77BCBEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{34F12B74-EAAA-4FAB-8E6A-C5FD1B6DE902}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>GRM033R71E103KE14D</t>
   </si>
@@ -396,9 +396,6 @@
     <t>https://www.mouser.fr/ProductDetail/Texas-Instruments/DSLVDS1048PWR?qs=%2Fha2pyFadui%2FTXskH3hgvdyHYEtJOlOyaJiQL0JEY3YjjG58Bx8NMDxqJeNgmMQY</t>
   </si>
   <si>
-    <t>U11, U12</t>
-  </si>
-  <si>
     <t>https://www.mouser.fr/ProductDetail/Texas-Instruments/TPS3703A7120DSERQ1?qs=%2Fha2pyFadui8P4qqv7wtJq7XkkCwOVhRNdsWZTFkD%252B34OV3EnMk3KZyek4uztLX0</t>
   </si>
   <si>
@@ -511,6 +508,18 @@
   </si>
   <si>
     <t>https://www.mouser.fr/ProductDetail/Murata-Electronics/KRM55WR71H336MH01L?qs=QzBtWTOodeWVwA4bjpST6w%3D%3D</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>TPS3703A7330DSERQ1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.fr/ProductDetail/Texas-Instruments/TPS3703A7330DSERQ1?qs=%2Fha2pyFadugGt5dAWQFWLSoN%2FsbubeOHv61%2FdlTbBouvNCowEjdZ9Q%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -913,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648BA62F-9DE5-4801-B4D1-F4154E9BA6E8}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +966,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1125,13 +1134,13 @@
         <v>64</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1183,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,13 +1234,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E18" s="5"/>
       <c r="G18" s="5"/>
@@ -1242,13 +1251,13 @@
         <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
@@ -1260,13 +1269,13 @@
         <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
@@ -1278,13 +1287,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1313,13 +1322,13 @@
         <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E23" s="4"/>
       <c r="G23" s="4"/>
@@ -1330,13 +1339,13 @@
         <v>74</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1344,13 +1353,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1425,7 +1434,7 @@
         <v>95</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1">
         <v>9</v>
@@ -1442,7 +1451,7 @@
         <v>96</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
@@ -1460,7 +1469,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -1476,7 +1485,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -1493,7 +1502,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -1509,7 +1518,7 @@
         <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C35" s="1">
         <v>7</v>
@@ -1527,7 +1536,7 @@
         <v>102</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -1545,7 +1554,7 @@
         <v>105</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C37" s="1">
         <v>10</v>
@@ -1563,7 +1572,7 @@
         <v>109</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C38" s="1">
         <v>7</v>
@@ -1599,7 +1608,7 @@
         <v>111</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1">
         <v>7</v>
@@ -1613,10 +1622,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
@@ -1765,83 +1774,99 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="C50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="E50" s="4"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" s="4"/>
-      <c r="G51" s="5"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>128</v>
+        <v>47</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E53" s="4"/>
-      <c r="G53" s="5"/>
+      <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>158</v>
+        <v>49</v>
       </c>
       <c r="C54" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="E54" s="4"/>
       <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="G55" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1894,12 +1919,13 @@
     <hyperlink ref="D48" r:id="rId47" xr:uid="{E9E3BCD4-C600-4E64-B407-73DDB6D25370}"/>
     <hyperlink ref="D49" r:id="rId48" xr:uid="{25F27107-4A1E-4CB2-96D2-8A405F105111}"/>
     <hyperlink ref="D50" r:id="rId49" xr:uid="{535BD460-1FA7-4312-91C5-B7FF64880C3B}"/>
-    <hyperlink ref="D51" r:id="rId50" xr:uid="{2269F43C-2242-4B95-964F-C2F23D9BCF3A}"/>
-    <hyperlink ref="D52" r:id="rId51" xr:uid="{028FDF0B-99DA-4968-B87D-E59F23E441BE}"/>
-    <hyperlink ref="D53" r:id="rId52" xr:uid="{BE46AE67-88D5-41B9-B027-72DDAD32EA3E}"/>
-    <hyperlink ref="D54" r:id="rId53" xr:uid="{BCC6C937-CED2-46E9-8EF0-088588498369}"/>
+    <hyperlink ref="D52" r:id="rId50" xr:uid="{2269F43C-2242-4B95-964F-C2F23D9BCF3A}"/>
+    <hyperlink ref="D53" r:id="rId51" xr:uid="{028FDF0B-99DA-4968-B87D-E59F23E441BE}"/>
+    <hyperlink ref="D54" r:id="rId52" xr:uid="{BE46AE67-88D5-41B9-B027-72DDAD32EA3E}"/>
+    <hyperlink ref="D55" r:id="rId53" xr:uid="{BCC6C937-CED2-46E9-8EF0-088588498369}"/>
+    <hyperlink ref="D51" r:id="rId54" xr:uid="{CC0BAACE-719A-4329-826B-42010321441C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>